<commit_message>
plugins and git project 27/03/25
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annep\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\annep\OneDrive\Desktop\git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB07CD07-879E-4021-B9BE-4A0479852A91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF200B9-7214-449C-91A0-438080BA6657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{54293126-1743-4F91-8A81-BCA292A51E93}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>S.NO</t>
   </si>
@@ -106,6 +106,21 @@
   </si>
   <si>
     <t>latest</t>
+  </si>
+  <si>
+    <t>jenkins/jenkins</t>
+  </si>
+  <si>
+    <t>6a44d1dd2d60</t>
+  </si>
+  <si>
+    <t>jenikins</t>
+  </si>
+  <si>
+    <t>cfb509230b4e</t>
+  </si>
+  <si>
+    <t>lts</t>
   </si>
 </sst>
 </file>
@@ -457,15 +472,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F6C4D45-742C-4A92-A740-EC1AEE175FF6}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.109375" customWidth="1"/>
@@ -572,6 +587,26 @@
         <v>23</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>